<commit_message>
modify Plan for phase 2
</commit_message>
<xml_diff>
--- a/Report_vers/.xlsx/Tasks.xlsx
+++ b/Report_vers/.xlsx/Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Elearning\HK232\Product_Classification_and_Delivery_Robot\Report_vers\.excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\E-learning\DACN\Product_Classification_and_Delivery_Robot\Report_vers\.xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A241ED-9536-460D-986B-52CCE762FD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1AB259-CD3C-4F6C-9811-0A14B8824068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sumary" sheetId="5" r:id="rId1"/>
@@ -19,26 +19,17 @@
     <sheet name="Hiện thực phần mềm" sheetId="3" r:id="rId4"/>
     <sheet name="Viết báo cáo" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -511,19 +502,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -532,9 +514,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -556,9 +535,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -569,50 +545,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -641,6 +584,54 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -930,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDB1B00-AA0F-4CAC-997C-7F39E9C1C3C6}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,99 +935,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="24" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="43">
+      <c r="A3" s="27">
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="31">
         <f>'Chuẩn bị cho khu vực test'!E10</f>
         <v>1</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="32">
         <f>C3/7</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="43">
+      <c r="A4" s="27">
         <v>2</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="31">
         <f>'Hiện thực phần cứng'!E24</f>
         <v>53</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="32">
         <f>C4/7</f>
         <v>7.5714285714285712</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="43">
+      <c r="A5" s="27">
         <v>3</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="31">
         <f>'Hiện thực phần mềm'!E24</f>
-        <v>51</v>
-      </c>
-      <c r="D5" s="48">
+        <v>44</v>
+      </c>
+      <c r="D5" s="32">
         <f>C5/7</f>
-        <v>7.2857142857142856</v>
+        <v>6.2857142857142856</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="45" t="s">
+      <c r="A6" s="27">
+        <v>4</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="31">
+        <f>'Viết báo cáo'!E5</f>
+        <v>7</v>
+      </c>
+      <c r="D6" s="32">
+        <f>C6/7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="15">
-        <f>SUM(C3:C5)</f>
+      <c r="C7" s="11">
+        <f>SUM(C3:C6)</f>
         <v>105</v>
       </c>
-      <c r="D6" s="42">
-        <f>C6/7</f>
+      <c r="D7" s="26">
+        <f>C7/7</f>
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="46" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C8" s="33">
         <v>105</v>
       </c>
-      <c r="D7" s="50">
-        <f>C7/7</f>
+      <c r="D8" s="34">
+        <f>C8/7</f>
         <v>15</v>
       </c>
     </row>
@@ -1054,7 +1061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7:E9"/>
     </sheetView>
   </sheetViews>
@@ -1074,146 +1081,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="40" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="5"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26">
+      <c r="A3" s="38">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="31" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="41">
         <v>0.2</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="14" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="39">
         <v>2</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="41">
         <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="14" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="40"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="39">
         <v>3</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="42">
         <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="14" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="14" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="40"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="29" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="25">
         <f>SUM(E3:E9)</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A9"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1224,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB87C40E-71C4-4476-A4A7-43D935245778}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F9"/>
+    <sheetView topLeftCell="B2" zoomScale="109" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,288 +1246,301 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="40" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="44">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="39">
         <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="17" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="17" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="39"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="15" t="s">
+      <c r="A7" s="45"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="15" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="15" t="s">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="44">
         <v>2</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="39">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="17" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="15" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="13" t="s">
+      <c r="A13" s="45"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="39">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="17" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="39"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="44">
         <v>3</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="39">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="17" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="17" t="s">
+      <c r="A17" s="45"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="13"/>
+      <c r="E17" s="39"/>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="13" t="s">
+      <c r="A18" s="45"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="39">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="17" t="s">
+      <c r="A19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="13"/>
+      <c r="E19" s="39"/>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="17" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="13"/>
+      <c r="E20" s="39"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="A21" s="39">
         <v>4</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="17" t="s">
+      <c r="C21" s="44"/>
+      <c r="D21" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="39">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="17" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="13"/>
+      <c r="E22" s="39"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="17" t="s">
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="13"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="20">
         <f>SUM(E3:E23)</f>
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A20"/>
@@ -1532,19 +1552,6 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="C21:C23"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1568,297 +1575,309 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="40" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="44">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="17" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="15" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="15" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="44">
         <v>2</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="39">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="17" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="17" t="s">
+      <c r="A10" s="45"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="24" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="24" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="24" t="s">
+      <c r="A13" s="45"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="15" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="44">
         <v>3</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="39">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="24" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13" t="s">
+      <c r="A17" s="45"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="39">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="24" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
+      <c r="A19" s="44">
         <v>4</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="24" t="s">
+      <c r="C19" s="44"/>
+      <c r="D19" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="39">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="24" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="13"/>
+      <c r="E20" s="39"/>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="A21" s="44">
         <v>5</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="13" t="s">
+      <c r="A22" s="45"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="13">
-        <v>14</v>
+      <c r="E22" s="39">
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="24" t="s">
+      <c r="A23" s="38"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="13"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="20" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="18">
         <f>SUM(E3:E23)</f>
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C25" s="19"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="E3:E5"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A23"/>
@@ -1870,21 +1889,9 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="B21:B23"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:A7"/>
     <mergeCell ref="A8:A14"/>
-    <mergeCell ref="E3:E5"/>
     <mergeCell ref="C8:C13"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="E19:E20"/>
     <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1908,63 +1915,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="40" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="50"/>
+      <c r="B2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="39">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="39">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="30" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <f>SUM(E3)</f>
         <v>7</v>
       </c>

</xml_diff>